<commit_message>
rewriting numpy to pandas dataframe
</commit_message>
<xml_diff>
--- a/TLMPortMapPlot/2024-07-01_17-16-37_MCR1_Rig1_cal_QR00169_1_20_3820_Bias_0_Override_7_29.50_45C/analysis/RFA gain, N = 1.xlsx
+++ b/TLMPortMapPlot/2024-07-01_17-16-37_MCR1_Rig1_cal_QR00169_1_20_3820_Bias_0_Override_7_29.50_45C/analysis/RFA gain, N = 1.xlsx
@@ -601,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.03299029592691364</v>
+        <v>0.0329902959269136</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -1095,7 +1095,7 @@
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>3.50125100612639</v>
+        <v>3.501251006126389</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -2311,7 +2311,7 @@
         <v>1</v>
       </c>
       <c r="D99" t="n">
-        <v>0.4015977959186579</v>
+        <v>0.4015977959186578</v>
       </c>
       <c r="E99" t="n">
         <v>0</v>
@@ -2330,7 +2330,7 @@
         <v>1</v>
       </c>
       <c r="D100" t="n">
-        <v>1.951021780508047</v>
+        <v>1.951021780508046</v>
       </c>
       <c r="E100" t="n">
         <v>0</v>
@@ -3033,7 +3033,7 @@
         <v>1</v>
       </c>
       <c r="D137" t="n">
-        <v>6.667137020401046</v>
+        <v>6.667137020401047</v>
       </c>
       <c r="E137" t="n">
         <v>0</v>
@@ -3413,7 +3413,7 @@
         <v>2</v>
       </c>
       <c r="D157" t="n">
-        <v>0.01909755462679305</v>
+        <v>0.019097554626793</v>
       </c>
       <c r="E157" t="n">
         <v>0</v>
@@ -3983,7 +3983,7 @@
         <v>2</v>
       </c>
       <c r="D187" t="n">
-        <v>0.238938369285315</v>
+        <v>0.2389383692853149</v>
       </c>
       <c r="E187" t="n">
         <v>0</v>
@@ -6700,7 +6700,7 @@
         <v>3</v>
       </c>
       <c r="D330" t="n">
-        <v>0.2154854549120569</v>
+        <v>0.2154854549120568</v>
       </c>
       <c r="E330" t="n">
         <v>0</v>
@@ -6928,7 +6928,7 @@
         <v>3</v>
       </c>
       <c r="D342" t="n">
-        <v>0.9442835801798827</v>
+        <v>0.9442835801798828</v>
       </c>
       <c r="E342" t="n">
         <v>0</v>
@@ -7935,7 +7935,7 @@
         <v>3</v>
       </c>
       <c r="D395" t="n">
-        <v>0.06087598009031726</v>
+        <v>0.0608759800903172</v>
       </c>
       <c r="E395" t="n">
         <v>0</v>
@@ -8334,7 +8334,7 @@
         <v>3</v>
       </c>
       <c r="D416" t="n">
-        <v>0.3763994126239729</v>
+        <v>0.3763994126239728</v>
       </c>
       <c r="E416" t="n">
         <v>0</v>
@@ -8714,7 +8714,7 @@
         <v>3</v>
       </c>
       <c r="D436" t="n">
-        <v>0.9441232930349829</v>
+        <v>0.9441232930349828</v>
       </c>
       <c r="E436" t="n">
         <v>0</v>
@@ -8885,7 +8885,7 @@
         <v>3</v>
       </c>
       <c r="D445" t="n">
-        <v>0.9205525519702389</v>
+        <v>0.9205525519702388</v>
       </c>
       <c r="E445" t="n">
         <v>0</v>

</xml_diff>